<commit_message>
code updated from stackoverflow
</commit_message>
<xml_diff>
--- a/Example input file submitted proposals.xlsx
+++ b/Example input file submitted proposals.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
-    <t xml:space="preserve">Application numbers</t>
+    <t xml:space="preserve">Application number</t>
   </si>
   <si>
     <t xml:space="preserve">Earth sciences</t>
@@ -158,8 +158,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -182,1020 +186,1020 @@
   </sheetPr>
   <dimension ref="A1:U1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A629" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A94" activeCellId="0" sqref="A94"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="0" t="n">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="0" t="n">
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="M5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="0" t="n">
+      <c r="M5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="G6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="0" t="n">
+      <c r="G6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="M7" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" s="0" t="n">
+      <c r="D9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="M10" s="0" t="n">
+      <c r="M10" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="M11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="R11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U11" s="0" t="n">
+      <c r="M11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U11" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="J13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M13" s="0" t="n">
+      <c r="J13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="0" t="n">
+      <c r="B14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="D15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="T15" s="0" t="n">
+      <c r="D15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T15" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="U16" s="0" t="n">
+      <c r="U16" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="J17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="0" t="n">
+      <c r="J17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="J18" s="0" t="n">
+      <c r="J18" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="0" t="n">
+      <c r="B19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="M20" s="0" t="n">
+      <c r="M20" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="M21" s="0" t="n">
+      <c r="M21" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="U22" s="0" t="n">
+      <c r="U22" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="J23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M23" s="0" t="n">
+      <c r="J23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M23" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="M24" s="0" t="n">
+      <c r="M24" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="M25" s="0" t="n">
+      <c r="M25" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+      <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="M26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="0" t="n">
+      <c r="M26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="D27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="T27" s="0" t="n">
+      <c r="D27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T27" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+      <c r="A28" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="G28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="T28" s="0" t="n">
+      <c r="G28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T28" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="H29" s="0" t="n">
+      <c r="H29" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+      <c r="A30" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="J30" s="0" t="n">
+      <c r="J30" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+      <c r="A31" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="H31" s="0" t="n">
+      <c r="H31" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+      <c r="A32" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="M32" s="0" t="n">
+      <c r="M32" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+      <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="M33" s="0" t="n">
+      <c r="M33" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+      <c r="A34" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
+      <c r="A35" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="D35" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J35" s="0" t="n">
+      <c r="D35" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J35" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
+      <c r="A36" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="H36" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M36" s="0" t="n">
+      <c r="H36" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M36" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+      <c r="A37" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="M37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q37" s="0" t="n">
+      <c r="M37" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
+      <c r="A38" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="M38" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q38" s="0" t="n">
+      <c r="M38" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
+      <c r="A39" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D39" s="0" t="n">
+      <c r="B39" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
+      <c r="A40" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="H40" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M40" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="R40" s="0" t="n">
+      <c r="H40" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M40" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R40" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
+      <c r="A41" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="M41" s="0" t="n">
+      <c r="M41" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
+      <c r="A42" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="H42" s="0" t="n">
+      <c r="H42" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
+      <c r="A43" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="D43" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J43" s="0" t="n">
+      <c r="D43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J43" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
+      <c r="A44" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D44" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L44" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q44" s="0" t="n">
+      <c r="B44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
+      <c r="A45" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="H45" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M45" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="R45" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U45" s="0" t="n">
+      <c r="H45" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M45" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R45" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U45" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
+      <c r="A46" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="D46" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q46" s="0" t="n">
+      <c r="D46" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q46" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
+      <c r="A47" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="D47" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J47" s="0" t="n">
+      <c r="D47" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J47" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
+      <c r="A48" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="G48" s="0" t="n">
+      <c r="G48" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
+      <c r="A49" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="M49" s="0" t="n">
+      <c r="M49" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="n">
+      <c r="A50" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="0" t="n">
+      <c r="B50" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
+      <c r="A51" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="D51" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H51" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J51" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L51" s="0" t="n">
+      <c r="D51" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H51" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J51" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L51" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="n">
+      <c r="A52" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="H52" s="0" t="n">
+      <c r="H52" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
+      <c r="A53" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="B53" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D53" s="0" t="n">
+      <c r="B53" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D53" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="n">
+      <c r="A54" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="H54" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U54" s="0" t="n">
+      <c r="H54" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U54" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="n">
+      <c r="A55" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="D55" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J55" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M55" s="0" t="n">
+      <c r="D55" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J55" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M55" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="n">
+      <c r="A56" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="H56" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q56" s="0" t="n">
+      <c r="H56" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q56" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="n">
+      <c r="A57" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="H57" s="0" t="n">
+      <c r="H57" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="n">
+      <c r="A58" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="D58" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J58" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M58" s="0" t="n">
+      <c r="D58" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J58" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M58" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="n">
+      <c r="A59" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="J59" s="0" t="n">
+      <c r="J59" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="n">
+      <c r="A60" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="B60" s="0" t="n">
+      <c r="B60" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
+      <c r="A61" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="M61" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q61" s="0" t="n">
+      <c r="M61" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q61" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="n">
+      <c r="A62" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="M62" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q62" s="0" t="n">
+      <c r="M62" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q62" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
+      <c r="A63" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="M63" s="0" t="n">
+      <c r="M63" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
+      <c r="A64" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="D64" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J64" s="0" t="n">
+      <c r="D64" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J64" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
+      <c r="A65" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="J65" s="0" t="n">
+      <c r="J65" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="n">
+      <c r="A66" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="D66" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G66" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J66" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L66" s="0" t="n">
+      <c r="D66" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G66" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J66" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L66" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="n">
+      <c r="A67" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="B67" s="0" t="n">
+      <c r="B67" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="n">
+      <c r="A68" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="M68" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q68" s="0" t="n">
+      <c r="M68" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q68" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="n">
+      <c r="A69" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="J69" s="0" t="n">
+      <c r="J69" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="n">
+      <c r="A70" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="M70" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="R70" s="0" t="n">
+      <c r="M70" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R70" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="n">
+      <c r="A71" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="J71" s="0" t="n">
+      <c r="J71" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="n">
+      <c r="A72" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="M72" s="0" t="n">
+      <c r="M72" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="n">
+      <c r="A73" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="J73" s="0" t="n">
+      <c r="J73" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="n">
+      <c r="A74" s="1" t="n">
         <v>73</v>
       </c>
-      <c r="D74" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J74" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L74" s="0" t="n">
+      <c r="D74" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J74" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L74" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="n">
+      <c r="A75" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="B75" s="0" t="n">
+      <c r="B75" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="n">
+      <c r="A76" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="D76" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J76" s="0" t="n">
+      <c r="D76" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J76" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="n">
+      <c r="A77" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="B77" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="R77" s="0" t="n">
+      <c r="B77" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R77" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="n">
+      <c r="A78" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="M78" s="0" t="n">
+      <c r="M78" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="n">
+      <c r="A79" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="R79" s="0" t="n">
+      <c r="R79" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="n">
+      <c r="A80" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="D80" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G80" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J80" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U80" s="0" t="n">
+      <c r="D80" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G80" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J80" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U80" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="n">
+      <c r="A81" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="H81" s="0" t="n">
+      <c r="H81" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="n">
+      <c r="A82" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="H82" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J82" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q82" s="0" t="n">
+      <c r="H82" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q82" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="n">
+      <c r="A83" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="J83" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M83" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q83" s="0" t="n">
+      <c r="J83" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M83" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q83" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="n">
+      <c r="A84" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="J84" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M84" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q84" s="0" t="n">
+      <c r="J84" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M84" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q84" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="n">
+      <c r="A85" s="1" t="n">
         <v>84</v>
       </c>
-      <c r="J85" s="0" t="n">
+      <c r="J85" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="n">
+      <c r="A86" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="J86" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M86" s="0" t="n">
+      <c r="J86" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M86" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="n">
+      <c r="A87" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="J87" s="0" t="n">
+      <c r="J87" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="n">
+      <c r="A88" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="M88" s="0" t="n">
+      <c r="M88" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="n">
+      <c r="A89" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="M89" s="0" t="n">
+      <c r="M89" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="n">
+      <c r="A90" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="M90" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q90" s="0" t="n">
+      <c r="M90" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q90" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="n">
+      <c r="A91" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="H91" s="0" t="n">
+      <c r="H91" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="n">
+      <c r="A92" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="B92" s="0" t="n">
+      <c r="B92" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="n">
+      <c r="A93" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="L93" s="0" t="n">
+      <c r="L93" s="1" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>